<commit_message>
:memo: updated documentation (a little) and fixed tests to reflect intended usage
</commit_message>
<xml_diff>
--- a/tests/test_vital_data.xlsx
+++ b/tests/test_vital_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakre/Code/dgc/WellcomeLeap/mhealth_feature_generation/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783F8CCA-1567-814D-9CEA-6B61450B7D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F60A230-36CE-8C4D-8EDE-BCA615019419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{8070E86D-E676-1547-B965-82D08C34C622}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>should be in non-sleep rest heart rate</t>
   </si>
   <si>
-    <t>ActiveEnergyBurned</t>
-  </si>
-  <si>
     <t>Apple Watch</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>body.quantity.count</t>
+  </si>
+  <si>
+    <t>AppleExerciseTime</t>
   </si>
 </sst>
 </file>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mmss\.\f"/>
+    <numFmt numFmtId="164" formatCode="mmss\.\f"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -166,7 +166,7 @@
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -190,9 +190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -336,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,10 +527,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
@@ -655,13 +655,13 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="J6" t="s">
         <v>20</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
       </c>
       <c r="K6">
         <v>1</v>

</xml_diff>